<commit_message>
Added integration with Regprecise Scraped data (excel Sheets)
</commit_message>
<xml_diff>
--- a/Capstone_regPrecise/genomes.xlsx
+++ b/Capstone_regPrecise/genomes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19620"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="19660"/>
   </bookViews>
   <sheets>
     <sheet name="Genomes" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="531">
   <si>
     <t>genomeId</t>
   </si>
@@ -68,9 +68,6 @@
     <t>343</t>
   </si>
   <si>
-    <t>345</t>
-  </si>
-  <si>
     <t>526</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>53</t>
   </si>
   <si>
-    <t>58</t>
-  </si>
-  <si>
     <t>60</t>
   </si>
   <si>
@@ -602,9 +596,6 @@
     <t>Aeromonas hydrophila subsp. hydrophila ATCC 7966</t>
   </si>
   <si>
-    <t>Aeromonas salmonicida subsp. salmonicida A449</t>
-  </si>
-  <si>
     <t>Aggregatibacter aphrophilus NJ8700</t>
   </si>
   <si>
@@ -656,9 +647,6 @@
     <t>Bacillus amyloliquefaciens FZB42</t>
   </si>
   <si>
-    <t>Bacillus cereus ATCC 14579</t>
-  </si>
-  <si>
     <t>Bacillus clausii KSM-K16</t>
   </si>
   <si>
@@ -1136,9 +1124,6 @@
     <t>380703</t>
   </si>
   <si>
-    <t>382245</t>
-  </si>
-  <si>
     <t>634176</t>
   </si>
   <si>
@@ -1188,9 +1173,6 @@
   </si>
   <si>
     <t>326423</t>
-  </si>
-  <si>
-    <t>226900</t>
   </si>
   <si>
     <t>66692</t>
@@ -1952,10 +1934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C179"/>
+  <dimension ref="A1:C177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
-      <selection activeCell="G173" sqref="G173"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1976,10 +1958,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1987,10 +1969,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1998,10 +1980,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2009,10 +1991,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C5" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2020,10 +2002,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C6" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2031,10 +2013,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C7" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2042,10 +2024,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C8" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2053,10 +2035,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C9" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2064,10 +2046,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C10" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2075,10 +2057,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C11" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2086,10 +2068,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C12" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2097,10 +2079,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C13" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2108,10 +2090,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C14" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2119,10 +2101,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C15" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -2130,10 +2112,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C16" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2141,10 +2123,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C17" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2152,10 +2134,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C18" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2163,10 +2145,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C19" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2174,10 +2156,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C20" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2185,10 +2167,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C21" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2196,10 +2178,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C22" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2207,10 +2189,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C23" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2218,10 +2200,10 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C24" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2229,10 +2211,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C25" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2240,10 +2222,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C26" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2251,10 +2233,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C27" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2262,10 +2244,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C28" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2273,10 +2255,10 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C29" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2284,10 +2266,10 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C30" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2295,10 +2277,10 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C31" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -2306,10 +2288,10 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C32" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2317,10 +2299,10 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C33" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -2328,10 +2310,10 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C34" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2339,10 +2321,10 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C35" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2350,10 +2332,10 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C36" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2361,10 +2343,10 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C37" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2372,10 +2354,10 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C38" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2383,10 +2365,10 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C39" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2394,10 +2376,10 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C40" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -2405,10 +2387,10 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C41" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -2416,10 +2398,10 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C42" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2427,10 +2409,10 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C43" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2438,10 +2420,10 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C44" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -2449,10 +2431,10 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C45" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -2460,10 +2442,10 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C46" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -2471,10 +2453,10 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C47" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -2482,10 +2464,10 @@
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C48" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -2493,10 +2475,10 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C49" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -2504,10 +2486,10 @@
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C50" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -2515,10 +2497,10 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C51" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -2526,10 +2508,10 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C52" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -2537,10 +2519,10 @@
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C53" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -2548,10 +2530,10 @@
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C54" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -2559,10 +2541,10 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C55" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -2570,10 +2552,10 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C56" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -2581,10 +2563,10 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C57" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -2592,10 +2574,10 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C58" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -2603,10 +2585,10 @@
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C59" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -2614,10 +2596,10 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C60" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -2625,10 +2607,10 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C61" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -2636,10 +2618,10 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C62" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -2647,10 +2629,10 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C63" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -2658,10 +2640,10 @@
         <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C64" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -2669,10 +2651,10 @@
         <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C65" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -2680,10 +2662,10 @@
         <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C66" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -2691,10 +2673,10 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C67" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -2702,10 +2684,10 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C68" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
@@ -2713,10 +2695,10 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C69" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -2724,10 +2706,10 @@
         <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C70" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -2735,10 +2717,10 @@
         <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C71" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -2746,10 +2728,10 @@
         <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C72" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -2757,10 +2739,10 @@
         <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C73" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -2768,10 +2750,10 @@
         <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C74" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -2779,10 +2761,10 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C75" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -2790,10 +2772,10 @@
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C76" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -2801,10 +2783,10 @@
         <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C77" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -2812,10 +2794,10 @@
         <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C78" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -2823,10 +2805,10 @@
         <v>80</v>
       </c>
       <c r="B79" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C79" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -2834,10 +2816,10 @@
         <v>81</v>
       </c>
       <c r="B80" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C80" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -2845,10 +2827,10 @@
         <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C81" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -2856,10 +2838,10 @@
         <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C82" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -2867,10 +2849,10 @@
         <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C83" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -2878,10 +2860,10 @@
         <v>85</v>
       </c>
       <c r="B84" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C84" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -2889,10 +2871,10 @@
         <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C85" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -2900,10 +2882,10 @@
         <v>87</v>
       </c>
       <c r="B86" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C86" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
@@ -2911,10 +2893,10 @@
         <v>88</v>
       </c>
       <c r="B87" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C87" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
@@ -2922,10 +2904,10 @@
         <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C88" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -2933,10 +2915,10 @@
         <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C89" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
@@ -2944,10 +2926,10 @@
         <v>91</v>
       </c>
       <c r="B90" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C90" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -2955,10 +2937,10 @@
         <v>92</v>
       </c>
       <c r="B91" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C91" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
@@ -2966,10 +2948,10 @@
         <v>93</v>
       </c>
       <c r="B92" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C92" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
@@ -2977,10 +2959,10 @@
         <v>94</v>
       </c>
       <c r="B93" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C93" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -2988,10 +2970,10 @@
         <v>95</v>
       </c>
       <c r="B94" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C94" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -2999,10 +2981,10 @@
         <v>96</v>
       </c>
       <c r="B95" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C95" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -3010,10 +2992,10 @@
         <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C96" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -3021,10 +3003,10 @@
         <v>98</v>
       </c>
       <c r="B97" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C97" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -3032,10 +3014,10 @@
         <v>99</v>
       </c>
       <c r="B98" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C98" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
@@ -3043,10 +3025,10 @@
         <v>100</v>
       </c>
       <c r="B99" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C99" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -3054,10 +3036,10 @@
         <v>101</v>
       </c>
       <c r="B100" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C100" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -3065,10 +3047,10 @@
         <v>102</v>
       </c>
       <c r="B101" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C101" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -3076,10 +3058,10 @@
         <v>103</v>
       </c>
       <c r="B102" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C102" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -3087,10 +3069,10 @@
         <v>104</v>
       </c>
       <c r="B103" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C103" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -3098,10 +3080,10 @@
         <v>105</v>
       </c>
       <c r="B104" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C104" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -3109,10 +3091,10 @@
         <v>106</v>
       </c>
       <c r="B105" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C105" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -3120,10 +3102,10 @@
         <v>107</v>
       </c>
       <c r="B106" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C106" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -3131,10 +3113,10 @@
         <v>108</v>
       </c>
       <c r="B107" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C107" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -3142,10 +3124,10 @@
         <v>109</v>
       </c>
       <c r="B108" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C108" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -3153,10 +3135,10 @@
         <v>110</v>
       </c>
       <c r="B109" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C109" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -3164,10 +3146,10 @@
         <v>111</v>
       </c>
       <c r="B110" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C110" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -3175,10 +3157,10 @@
         <v>112</v>
       </c>
       <c r="B111" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C111" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -3186,10 +3168,10 @@
         <v>113</v>
       </c>
       <c r="B112" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C112" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -3197,10 +3179,10 @@
         <v>114</v>
       </c>
       <c r="B113" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C113" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -3208,10 +3190,10 @@
         <v>115</v>
       </c>
       <c r="B114" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C114" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -3219,10 +3201,10 @@
         <v>116</v>
       </c>
       <c r="B115" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C115" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -3230,10 +3212,10 @@
         <v>117</v>
       </c>
       <c r="B116" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C116" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -3241,10 +3223,10 @@
         <v>118</v>
       </c>
       <c r="B117" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C117" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -3252,10 +3234,10 @@
         <v>119</v>
       </c>
       <c r="B118" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C118" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -3263,10 +3245,10 @@
         <v>120</v>
       </c>
       <c r="B119" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C119" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -3274,10 +3256,10 @@
         <v>121</v>
       </c>
       <c r="B120" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C120" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -3285,10 +3267,10 @@
         <v>122</v>
       </c>
       <c r="B121" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C121" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -3296,10 +3278,10 @@
         <v>123</v>
       </c>
       <c r="B122" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C122" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
@@ -3307,10 +3289,10 @@
         <v>124</v>
       </c>
       <c r="B123" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C123" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
@@ -3318,10 +3300,10 @@
         <v>125</v>
       </c>
       <c r="B124" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C124" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
@@ -3329,10 +3311,10 @@
         <v>126</v>
       </c>
       <c r="B125" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C125" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
@@ -3340,10 +3322,10 @@
         <v>127</v>
       </c>
       <c r="B126" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C126" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
@@ -3351,10 +3333,10 @@
         <v>128</v>
       </c>
       <c r="B127" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C127" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
@@ -3362,10 +3344,10 @@
         <v>129</v>
       </c>
       <c r="B128" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C128" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
@@ -3373,10 +3355,10 @@
         <v>130</v>
       </c>
       <c r="B129" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C129" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
@@ -3384,10 +3366,10 @@
         <v>131</v>
       </c>
       <c r="B130" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C130" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
@@ -3395,10 +3377,10 @@
         <v>132</v>
       </c>
       <c r="B131" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C131" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
@@ -3406,10 +3388,10 @@
         <v>133</v>
       </c>
       <c r="B132" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C132" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
@@ -3417,10 +3399,10 @@
         <v>134</v>
       </c>
       <c r="B133" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C133" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
@@ -3428,10 +3410,10 @@
         <v>135</v>
       </c>
       <c r="B134" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C134" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
@@ -3439,10 +3421,10 @@
         <v>136</v>
       </c>
       <c r="B135" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C135" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
@@ -3450,10 +3432,10 @@
         <v>137</v>
       </c>
       <c r="B136" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C136" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
@@ -3461,10 +3443,10 @@
         <v>138</v>
       </c>
       <c r="B137" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C137" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
@@ -3472,10 +3454,10 @@
         <v>139</v>
       </c>
       <c r="B138" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C138" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
@@ -3483,10 +3465,10 @@
         <v>140</v>
       </c>
       <c r="B139" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C139" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
@@ -3494,10 +3476,10 @@
         <v>141</v>
       </c>
       <c r="B140" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C140" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
@@ -3505,10 +3487,10 @@
         <v>142</v>
       </c>
       <c r="B141" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C141" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
@@ -3516,10 +3498,10 @@
         <v>143</v>
       </c>
       <c r="B142" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C142" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
@@ -3527,10 +3509,10 @@
         <v>144</v>
       </c>
       <c r="B143" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C143" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
@@ -3538,10 +3520,10 @@
         <v>145</v>
       </c>
       <c r="B144" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C144" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
@@ -3549,10 +3531,10 @@
         <v>146</v>
       </c>
       <c r="B145" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C145" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
@@ -3560,10 +3542,10 @@
         <v>147</v>
       </c>
       <c r="B146" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C146" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
@@ -3571,10 +3553,10 @@
         <v>148</v>
       </c>
       <c r="B147" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C147" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
@@ -3582,10 +3564,10 @@
         <v>149</v>
       </c>
       <c r="B148" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C148" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
@@ -3593,10 +3575,10 @@
         <v>150</v>
       </c>
       <c r="B149" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C149" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
@@ -3604,10 +3586,10 @@
         <v>151</v>
       </c>
       <c r="B150" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C150" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
@@ -3615,10 +3597,10 @@
         <v>152</v>
       </c>
       <c r="B151" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C151" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
@@ -3626,10 +3608,10 @@
         <v>153</v>
       </c>
       <c r="B152" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C152" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
@@ -3637,10 +3619,10 @@
         <v>154</v>
       </c>
       <c r="B153" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C153" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
@@ -3648,10 +3630,10 @@
         <v>155</v>
       </c>
       <c r="B154" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C154" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
@@ -3659,10 +3641,10 @@
         <v>156</v>
       </c>
       <c r="B155" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C155" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
@@ -3670,10 +3652,10 @@
         <v>157</v>
       </c>
       <c r="B156" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C156" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
@@ -3681,10 +3663,10 @@
         <v>158</v>
       </c>
       <c r="B157" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C157" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
@@ -3692,10 +3674,10 @@
         <v>159</v>
       </c>
       <c r="B158" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C158" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
@@ -3703,10 +3685,10 @@
         <v>160</v>
       </c>
       <c r="B159" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C159" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
@@ -3714,10 +3696,10 @@
         <v>161</v>
       </c>
       <c r="B160" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C160" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
@@ -3725,10 +3707,10 @@
         <v>162</v>
       </c>
       <c r="B161" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C161" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
@@ -3736,10 +3718,10 @@
         <v>163</v>
       </c>
       <c r="B162" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C162" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
@@ -3747,10 +3729,10 @@
         <v>164</v>
       </c>
       <c r="B163" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C163" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
@@ -3758,10 +3740,10 @@
         <v>165</v>
       </c>
       <c r="B164" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C164" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
@@ -3769,10 +3751,10 @@
         <v>166</v>
       </c>
       <c r="B165" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C165" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
@@ -3780,10 +3762,10 @@
         <v>167</v>
       </c>
       <c r="B166" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C166" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
@@ -3791,10 +3773,10 @@
         <v>168</v>
       </c>
       <c r="B167" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C167" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
@@ -3802,10 +3784,10 @@
         <v>169</v>
       </c>
       <c r="B168" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C168" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
@@ -3813,10 +3795,10 @@
         <v>170</v>
       </c>
       <c r="B169" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C169" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
@@ -3824,10 +3806,10 @@
         <v>171</v>
       </c>
       <c r="B170" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C170" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
@@ -3835,10 +3817,10 @@
         <v>172</v>
       </c>
       <c r="B171" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C171" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
@@ -3846,10 +3828,10 @@
         <v>173</v>
       </c>
       <c r="B172" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C172" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
@@ -3857,10 +3839,10 @@
         <v>174</v>
       </c>
       <c r="B173" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C173" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
@@ -3868,10 +3850,10 @@
         <v>175</v>
       </c>
       <c r="B174" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C174" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
@@ -3879,10 +3861,10 @@
         <v>176</v>
       </c>
       <c r="B175" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C175" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
@@ -3890,10 +3872,10 @@
         <v>177</v>
       </c>
       <c r="B176" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C176" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
@@ -3901,32 +3883,10 @@
         <v>178</v>
       </c>
       <c r="B177" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C177" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A178" t="s">
-        <v>179</v>
-      </c>
-      <c r="B178" t="s">
-        <v>357</v>
-      </c>
-      <c r="C178" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A179" t="s">
-        <v>180</v>
-      </c>
-      <c r="B179" t="s">
-        <v>358</v>
-      </c>
-      <c r="C179" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
   </sheetData>

</xml_diff>